<commit_message>
Bug fix: ImmobilizeEndGame was using "not any" of moves which would mistakenly end a game on South's turn if their only move was from the leftmost hole. Bug fix: board setup was using eliminate instead of show_seeds_in_stores, preventing setup for games like Azigo. Azigo board size changed to 14 (20 is still a variation). Unit test coverages back to 100%.
</commit_message>
<xml_diff>
--- a/analysis/data/worksheet_combine.xlsx
+++ b/analysis/data/worksheet_combine.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Activity_Data\Mancala_github\MancalaGames\analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8505610-E253-4BA8-8462-05BACE73356A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17867669-B8ED-4840-8472-CBCD37362A48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29580" yWindow="780" windowWidth="25410" windowHeight="14265" xr2:uid="{9656757A-5440-4F99-A97B-B1C6A0885C28}"/>
+    <workbookView xWindow="31140" yWindow="1935" windowWidth="25410" windowHeight="14265" xr2:uid="{9656757A-5440-4F99-A97B-B1C6A0885C28}"/>
   </bookViews>
   <sheets>
     <sheet name="combine 1" sheetId="1" r:id="rId1"/>
@@ -215,24 +215,31 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="44">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+  <dxfs count="46">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.749961851863155"/>
         </patternFill>
       </fill>
     </dxf>
@@ -254,23 +261,6 @@
       <fill>
         <patternFill>
           <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.749961851863155"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -312,11 +302,31 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -338,16 +348,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -384,26 +384,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -424,6 +404,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -559,6 +559,20 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.749961851863155"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1009,8 +1023,8 @@
   </sheetPr>
   <dimension ref="A1:AD13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:K6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1315,45 +1329,55 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:C3">
-    <cfRule type="cellIs" dxfId="43" priority="138" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="45" priority="140" operator="greaterThan">
       <formula>1000</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B5:C6">
-    <cfRule type="cellIs" dxfId="42" priority="1" operator="greaterThan">
+  <conditionalFormatting sqref="B5:C5">
+    <cfRule type="cellIs" dxfId="44" priority="3" operator="greaterThan">
       <formula>1000</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="43" priority="4" operator="greaterThan">
       <formula>5000</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3:P3">
-    <cfRule type="cellIs" dxfId="40" priority="131" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="42" priority="133" stopIfTrue="1" operator="lessThan">
       <formula>0.4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="132" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="41" priority="134" stopIfTrue="1" operator="greaterThan">
       <formula>0.6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="133" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="40" priority="135" stopIfTrue="1" operator="lessThan">
       <formula>0.48</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="134" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="39" priority="136" operator="greaterThan">
       <formula>0.52</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q3">
-    <cfRule type="cellIs" dxfId="36" priority="128" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="38" priority="130" operator="greaterThan">
       <formula>0.4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="129" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="37" priority="131" stopIfTrue="1" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="130" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="36" priority="132" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="X3:Y3">
+    <cfRule type="cellIs" dxfId="35" priority="1" operator="between">
+      <formula>0.05</formula>
+      <formula>0.15</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="2" operator="between">
+      <formula>0.001</formula>
+      <formula>0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="AA3:AB3">
-    <cfRule type="cellIs" dxfId="33" priority="139" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="141" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1369,7 +1393,7 @@
   <dimension ref="A1:AD26"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1921,17 +1945,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O20:P20">
-    <cfRule type="cellIs" dxfId="19" priority="30" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="19" priority="27" stopIfTrue="1" operator="lessThan">
+      <formula>0.4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="28" stopIfTrue="1" operator="greaterThan">
+      <formula>0.6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="29" stopIfTrue="1" operator="lessThan">
+      <formula>0.48</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="30" operator="greaterThan">
       <formula>0.52</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="29" stopIfTrue="1" operator="lessThan">
-      <formula>0.48</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="28" stopIfTrue="1" operator="greaterThan">
-      <formula>0.6</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="27" stopIfTrue="1" operator="lessThan">
-      <formula>0.4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P5">
@@ -1946,25 +1970,25 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q3">
-    <cfRule type="cellIs" dxfId="12" priority="34" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="33" operator="greaterThan">
+      <formula>0.4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="34" stopIfTrue="1" operator="greaterThan">
       <formula>0.1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="33" operator="greaterThan">
-      <formula>0.4</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="10" priority="35" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q20">
-    <cfRule type="cellIs" dxfId="9" priority="26" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="25" stopIfTrue="1" operator="greaterThan">
+      <formula>0.1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="26" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="24" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="24" operator="greaterThan">
       <formula>0.4</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="25" stopIfTrue="1" operator="greaterThan">
-      <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S5:T5">
@@ -1973,23 +1997,23 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X3:Y3">
-    <cfRule type="cellIs" dxfId="5" priority="22" operator="between">
+    <cfRule type="cellIs" dxfId="5" priority="21" operator="between">
+      <formula>0.05</formula>
+      <formula>0.15</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="22" operator="between">
       <formula>0.001</formula>
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="21" operator="between">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X20:Y20">
+    <cfRule type="cellIs" dxfId="3" priority="19" operator="between">
       <formula>0.05</formula>
       <formula>0.15</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X20:Y20">
-    <cfRule type="cellIs" dxfId="3" priority="20" operator="between">
+    <cfRule type="cellIs" dxfId="2" priority="20" operator="between">
       <formula>0.001</formula>
       <formula>0.05</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="19" operator="between">
-      <formula>0.05</formula>
-      <formula>0.15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA3:AB3">

</xml_diff>